<commit_message>
Updated units for bosnia; updated weights for bosnia; updated weights for netherlands; updated omega 3 code and files for brazil
</commit_message>
<xml_diff>
--- a/data/raw/Brazil/brazil_ingredients_trans_dha_epa.xlsx
+++ b/data/raw/Brazil/brazil_ingredients_trans_dha_epa.xlsx
@@ -1,32 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrisunjae/Documents/Activities/Golden Research/subnational_distributions/data/raw/Brazil/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Simone/Dropbox/Github/subnational_distributions/data/raw/Brazil/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{747FBBCB-6A85-CA45-8D08-25679848184E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC2F0E8-BBF9-554D-A6A5-14DA474D0C72}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22920" yWindow="500" windowWidth="22920" windowHeight="28300"/>
+    <workbookView xWindow="28800" yWindow="-220" windowWidth="22920" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="brazil_ingredients_trans_dha_ep" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -552,9 +541,6 @@
     <t>Used FDC: Crab salad made with imitation crab</t>
   </si>
   <si>
-    <t>No info found</t>
-  </si>
-  <si>
     <t>Used FDC: Shrimp soup, cream of, prepared with water</t>
   </si>
   <si>
@@ -562,12 +548,15 @@
   </si>
   <si>
     <t>Used FDC: Sea bass, steamed or poached</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/229965981_Fatty_acid_composition_in_wild_and_cultivated_pacu_and_pintado_fish</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.###;;"/>
   </numFmts>
@@ -1415,14 +1404,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="51.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -2061,11 +2053,10 @@
         <v>46</v>
       </c>
       <c r="I20" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.956</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -2088,11 +2079,10 @@
         <v>47</v>
       </c>
       <c r="I21" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.956</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -2415,7 +2405,7 @@
         <v>0</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
@@ -2512,7 +2502,7 @@
         <v>0.51500000000000001</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
@@ -2545,7 +2535,7 @@
         <v>0.748</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
@@ -3601,7 +3591,7 @@
         <v>0.121</v>
       </c>
       <c r="I68" s="1">
-        <f t="shared" ref="I66:I74" si="10">G68+H68</f>
+        <f t="shared" ref="I68:I74" si="10">G68+H68</f>
         <v>0.16399999999999998</v>
       </c>
       <c r="J68" t="s">

</xml_diff>